<commit_message>
Update CDI final report
</commit_message>
<xml_diff>
--- a/badbaby/static/cdi_report_final_08292018.xlsx
+++ b/badbaby/static/cdi_report_final_08292018.xlsx
@@ -587,8 +587,8 @@
   </sheetPr>
   <dimension ref="A1:AC348"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F122" activeCellId="0" sqref="F122"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A140" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F158" activeCellId="0" sqref="F158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14590,7 +14590,7 @@
         <v>32</v>
       </c>
       <c r="F158" s="0" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G158" s="0" t="n">
         <v>31</v>
@@ -31591,7 +31591,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="1" sqref="F122 E23"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="1" sqref="F158 E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>